<commit_message>
added near failure function
</commit_message>
<xml_diff>
--- a/backend/app/mod_gate/static/闸机上传模版.xlsx
+++ b/backend/app/mod_gate/static/闸机上传模版.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/desmond/Repos/quatek_web_app_project/backend/app/mod_gate/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CE12C29-2C43-604B-8761-83623A58FC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48283BCB-8286-AC46-B02A-67BFBFE5968F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="1860" windowWidth="28240" windowHeight="17440" xr2:uid="{F772C2DB-13A7-864E-9F57-DAD8663E0AF8}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>*gate_name</t>
   </si>
@@ -79,13 +79,25 @@
   </si>
   <si>
     <t>gate_port</t>
+  </si>
+  <si>
+    <t>hand_near_max</t>
+  </si>
+  <si>
+    <t>hand_near_min</t>
+  </si>
+  <si>
+    <t>foot_near_max</t>
+  </si>
+  <si>
+    <t>foot_near_min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +112,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,8 +143,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -446,9 +468,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{624EBA1C-EE16-A24C-A5AE-600123DA5E21}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -463,7 +487,7 @@
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,6 +517,18 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>